<commit_message>
Update descriptive analysis and formatted tables
</commit_message>
<xml_diff>
--- a/01. Descriptives/out/Table 3.xlsx
+++ b/01. Descriptives/out/Table 3.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="12">
   <si>
     <t>Año</t>
   </si>
@@ -21,10 +21,19 @@
     <t>Colectivo</t>
   </si>
   <si>
+    <t>Hombres</t>
+  </si>
+  <si>
     <t>Mujeres</t>
   </si>
   <si>
+    <t>Español</t>
+  </si>
+  <si>
     <t>Extranjeros</t>
+  </si>
+  <si>
+    <t>Mayores de 30</t>
   </si>
   <si>
     <t>Jóvenes</t>
@@ -85,7 +94,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D25"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -96,10 +105,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
@@ -110,10 +119,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1">
-        <v>52.160079956054688</v>
+        <v>47.839920043945313</v>
       </c>
     </row>
     <row r="3">
@@ -124,10 +133,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
-        <v>53.789634704589844</v>
+        <v>46.210365295410156</v>
       </c>
     </row>
     <row r="4">
@@ -138,10 +147,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1">
-        <v>13.660950660705566</v>
+        <v>52.160079956054688</v>
       </c>
     </row>
     <row r="5">
@@ -152,10 +161,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1">
-        <v>13.996814727783203</v>
+        <v>53.789634704589844</v>
       </c>
     </row>
     <row r="6">
@@ -166,10 +175,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1">
-        <v>24.216415405273438</v>
+        <v>86.33905029296875</v>
       </c>
     </row>
     <row r="7">
@@ -180,93 +189,261 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1">
-        <v>25.245389938354492</v>
+        <v>86.003181457519531</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1">
-        <v>52.376182556152344</v>
+        <v>13.660950660705566</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1">
-        <v>53.983905792236328</v>
+        <v>13.996814727783203</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D10" s="1">
-        <v>15.007454872131348</v>
+        <v>75.783584594726563</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1">
-        <v>15.350111961364746</v>
+        <v>74.754608154296875</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1">
-        <v>26.773412704467773</v>
+        <v>24.216415405273438</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1">
+        <v>25.245389938354492</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="1">
+        <v>47.623817443847656</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1">
+        <v>46.016094207763672</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="1">
+        <v>52.376182556152344</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1">
+        <v>53.983905792236328</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="1">
+        <v>84.992546081542969</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1">
+        <v>84.649887084960938</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="1">
+        <v>15.007454872131348</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1">
+        <v>15.350111961364746</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1">
+        <v>73.226585388183594</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="1">
+        <v>72.2049560546875</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B24" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="1">
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1">
+        <v>26.773412704467773</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="1">
         <v>27.7950439453125</v>
       </c>
     </row>

</xml_diff>